<commit_message>
Retrieve all row data for specific cell
</commit_message>
<xml_diff>
--- a/xlsx/libro.xlsx
+++ b/xlsx/libro.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Camilo\Desktop\python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Camilo\Desktop\python\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12288" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12288" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>ID</t>
   </si>
@@ -38,6 +38,36 @@
   </si>
   <si>
     <t>Holaa hojita 2</t>
+  </si>
+  <si>
+    <t>Juli</t>
+  </si>
+  <si>
+    <t>Ruiz</t>
+  </si>
+  <si>
+    <t>Andres</t>
+  </si>
+  <si>
+    <t>Rincon</t>
+  </si>
+  <si>
+    <t>Edad</t>
+  </si>
+  <si>
+    <t>Estado</t>
+  </si>
+  <si>
+    <t>Altura</t>
+  </si>
+  <si>
+    <t>Soltero</t>
+  </si>
+  <si>
+    <t>Soltera</t>
+  </si>
+  <si>
+    <t>Casado</t>
   </si>
 </sst>
 </file>
@@ -377,13 +407,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -393,8 +425,17 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2</v>
       </c>
@@ -404,27 +445,54 @@
       <c r="C2" t="s">
         <v>4</v>
       </c>
+      <c r="D2">
+        <v>24</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2">
+        <v>1.7</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>7</v>
+      </c>
+      <c r="D3">
+        <v>23</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3">
+        <v>1.71</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
+        <v>9</v>
+      </c>
+      <c r="D4">
+        <v>22</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4">
+        <v>1.5</v>
       </c>
     </row>
   </sheetData>
@@ -436,8 +504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9B66363-DB0B-41F6-8C35-B9DF809C65DA}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>